<commit_message>
:sparkles: se finaliza bot de creacion de excel reels
</commit_message>
<xml_diff>
--- a/excel_campañas/Reels_botanica_indio_amazonico - copia.xlsx
+++ b/excel_campañas/Reels_botanica_indio_amazonico - copia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DESARROLLADOR\Documents\Manuel Cardona\bot_reels_excel_communitys\excel_campañas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704D485F-9DDB-4D35-B9F3-DD577D4FC189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F320970-3888-4669-B776-FB02B9586736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -214,13 +214,13 @@
     <t>https://drive.google.com/file/d/1ZluPIdfgH_GXQoNElnuW7OAwjtoFPVp7/view</t>
   </si>
   <si>
-    <t>03:00:00 PM</t>
+    <t>Autocomentarse</t>
   </si>
   <si>
-    <t>08:00:00 PM</t>
+    <t>15:00</t>
   </si>
   <si>
-    <t>Autocomentarse</t>
+    <t>20:00</t>
   </si>
 </sst>
 </file>
@@ -546,7 +546,7 @@
   <dimension ref="A1:BD969"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AQ3" sqref="AQ3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -726,10 +726,10 @@
         <v>60</v>
       </c>
       <c r="B2" s="8">
-        <v>45787</v>
+        <v>45790</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D2" s="10" t="b">
         <v>0</v>
@@ -815,7 +815,7 @@
         <v>1</v>
       </c>
       <c r="AQ2" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="AR2" s="2">
         <v>1</v>
@@ -852,10 +852,10 @@
         <v>62</v>
       </c>
       <c r="B3" s="8">
-        <v>45788</v>
+        <v>45791</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D3" s="10" t="b">
         <v>0</v>
@@ -941,7 +941,7 @@
         <v>2</v>
       </c>
       <c r="AQ3" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="AR3" s="2">
         <v>2</v>

</xml_diff>